<commit_message>
udated protokolln geogebra file
</commit_message>
<xml_diff>
--- a/Stereoaufnahmen_Anja/protokoll.xlsx
+++ b/Stereoaufnahmen_Anja/protokoll.xlsx
@@ -143,13 +143,13 @@
     <t>K in mm (transponiert)</t>
   </si>
   <si>
-    <t>150-160 mm (+)</t>
-  </si>
-  <si>
-    <t>ca 0,5 mm (-)</t>
-  </si>
-  <si>
-    <t>ca 55 mm(-)</t>
+    <t>150-160 cm (+)</t>
+  </si>
+  <si>
+    <t>ca 1 cm (-)</t>
+  </si>
+  <si>
+    <t>ca 55 cm(-)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added matlab stereocalibration and m files for tests
</commit_message>
<xml_diff>
--- a/Stereoaufnahmen_Anja/protokoll.xlsx
+++ b/Stereoaufnahmen_Anja/protokoll.xlsx
@@ -146,10 +146,10 @@
     <t>150-160 cm (+)</t>
   </si>
   <si>
-    <t>ca 1 cm (-)</t>
-  </si>
-  <si>
-    <t>ca 55 cm(-)</t>
+    <t>ca 50 - 55 cm(-)</t>
+  </si>
+  <si>
+    <t>ca 0,7 - 1 cm (-)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="J22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>